<commit_message>
Added saving original clip
</commit_message>
<xml_diff>
--- a/dummy.xlsx
+++ b/dummy.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -407,6 +407,14 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="C1" t="n">
+        <v>5244.444444444444</v>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>CK1_1_0002.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -417,12 +425,28 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="C2" t="n">
+        <v>1662.698412698413</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CK1_1_0002.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>3481.746031746031</v>
       </c>
       <c r="B3" t="inlineStr">
+        <is>
+          <t>CK1_1_0002.jpg</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>7256.349206349206</v>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>CK1_1_0002.jpg</t>
         </is>

</xml_diff>

<commit_message>
filling algorithm had a bug
</commit_message>
<xml_diff>
--- a/dummy.xlsx
+++ b/dummy.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:X79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,6 +439,62 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="K1" t="n">
+        <v>12974.60317460317</v>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>S-CTL4-2_0012.jpg</t>
+        </is>
+      </c>
+      <c r="M1" t="n">
+        <v>1290.47619047619</v>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>CK1_1_0002.jpg</t>
+        </is>
+      </c>
+      <c r="O1" t="n">
+        <v>8124.603174603174</v>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="Q1" t="n">
+        <v>16143.65079365079</v>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S1" t="n">
+        <v>1034.920634920635</v>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="U1" t="n">
+        <v>8226.190476190475</v>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
+      <c r="W1" t="n">
+        <v>4141.269841269841</v>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -481,6 +537,38 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="K2" t="n">
+        <v>929.3650793650793</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>S-CTL4-2_0012.jpg</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>3310.31746031746</v>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S2" t="n">
+        <v>5288.888888888889</v>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W2" t="n">
+        <v>6569.841269841269</v>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -523,6 +611,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q3" t="n">
+        <v>3943.650793650793</v>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S3" t="n">
+        <v>5149.206349206349</v>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W3" t="n">
+        <v>5138.095238095238</v>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -557,6 +669,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q4" t="n">
+        <v>4169.047619047619</v>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S4" t="n">
+        <v>6040.47619047619</v>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W4" t="n">
+        <v>5316.666666666666</v>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -591,6 +727,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q5" t="n">
+        <v>2944.444444444444</v>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S5" t="n">
+        <v>2973.809523809524</v>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W5" t="n">
+        <v>8216.666666666666</v>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -625,6 +785,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q6" t="n">
+        <v>7067.460317460317</v>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S6" t="n">
+        <v>7641.269841269841</v>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W6" t="n">
+        <v>3866.666666666667</v>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="E7" t="n">
@@ -651,6 +835,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q7" t="n">
+        <v>4610.31746031746</v>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S7" t="n">
+        <v>4860.31746031746</v>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W7" t="n">
+        <v>7185.714285714285</v>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="E8" t="n">
@@ -677,6 +885,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q8" t="n">
+        <v>2933.333333333333</v>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S8" t="n">
+        <v>5451.587301587301</v>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W8" t="n">
+        <v>7470.63492063492</v>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="E9" t="n">
@@ -703,6 +935,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q9" t="n">
+        <v>5918.253968253968</v>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S9" t="n">
+        <v>8925.396825396825</v>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W9" t="n">
+        <v>1750</v>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="E10" t="n">
@@ -729,6 +985,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q10" t="n">
+        <v>2248.412698412698</v>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S10" t="n">
+        <v>14431.74603174603</v>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W10" t="n">
+        <v>4158.730158730158</v>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="E11" t="n">
@@ -755,6 +1035,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q11" t="n">
+        <v>7923.015873015873</v>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S11" t="n">
+        <v>13357.93650793651</v>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W11" t="n">
+        <v>5001.587301587301</v>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="E12" t="n">
@@ -781,6 +1085,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q12" t="n">
+        <v>7842.063492063492</v>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S12" t="n">
+        <v>18054.7619047619</v>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W12" t="n">
+        <v>4379.36507936508</v>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="E13" t="n">
@@ -807,6 +1135,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q13" t="n">
+        <v>8415.873015873016</v>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S13" t="n">
+        <v>7863.492063492063</v>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W13" t="n">
+        <v>4183.333333333333</v>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="E14" t="n">
@@ -833,6 +1185,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q14" t="n">
+        <v>2719.84126984127</v>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S14" t="n">
+        <v>6634.920634920634</v>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W14" t="n">
+        <v>2888.888888888889</v>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="E15" t="n">
@@ -859,6 +1235,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q15" t="n">
+        <v>3612.698412698413</v>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S15" t="n">
+        <v>16443.65079365079</v>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W15" t="n">
+        <v>4601.587301587301</v>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="E16" t="n">
@@ -885,6 +1285,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q16" t="n">
+        <v>5277.777777777777</v>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S16" t="n">
+        <v>4271.428571428572</v>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W16" t="n">
+        <v>7130.952380952381</v>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="E17" t="n">
@@ -911,6 +1335,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q17" t="n">
+        <v>4069.047619047619</v>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S17" t="n">
+        <v>7922.222222222222</v>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W17" t="n">
+        <v>3975.396825396825</v>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="E18" t="n">
@@ -937,6 +1385,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q18" t="n">
+        <v>2719.84126984127</v>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S18" t="n">
+        <v>8099.206349206349</v>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W18" t="n">
+        <v>12307.14285714286</v>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="E19" t="n">
@@ -963,6 +1435,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q19" t="n">
+        <v>11930.95238095238</v>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S19" t="n">
+        <v>5346.031746031746</v>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W19" t="n">
+        <v>2531.746031746032</v>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="E20" t="n">
@@ -989,6 +1485,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q20" t="n">
+        <v>6613.492063492063</v>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S20" t="n">
+        <v>1707.142857142857</v>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W20" t="n">
+        <v>3807.142857142857</v>
+      </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="E21" t="n">
@@ -1015,6 +1535,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q21" t="n">
+        <v>2693.650793650793</v>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S21" t="n">
+        <v>12568.25396825397</v>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W21" t="n">
+        <v>7168.253968253968</v>
+      </c>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="E22" t="n">
@@ -1041,6 +1585,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q22" t="n">
+        <v>2108.730158730159</v>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S22" t="n">
+        <v>6311.904761904761</v>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W22" t="n">
+        <v>7091.269841269841</v>
+      </c>
+      <c r="X22" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="E23" t="n">
@@ -1067,6 +1635,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q23" t="n">
+        <v>10019.84126984127</v>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S23" t="n">
+        <v>6461.904761904761</v>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W23" t="n">
+        <v>8177.777777777777</v>
+      </c>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="E24" t="n">
@@ -1093,6 +1685,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q24" t="n">
+        <v>3608.730158730159</v>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S24" t="n">
+        <v>1772.222222222222</v>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W24" t="n">
+        <v>5373.015873015873</v>
+      </c>
+      <c r="X24" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="E25" t="n">
@@ -1119,6 +1735,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q25" t="n">
+        <v>9918.253968253968</v>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S25" t="n">
+        <v>3935.714285714285</v>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W25" t="n">
+        <v>8712.698412698412</v>
+      </c>
+      <c r="X25" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="E26" t="n">
@@ -1145,6 +1785,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q26" t="n">
+        <v>4476.190476190476</v>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S26" t="n">
+        <v>6107.142857142857</v>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W26" t="n">
+        <v>909.5238095238095</v>
+      </c>
+      <c r="X26" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="E27" t="n">
@@ -1171,6 +1835,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q27" t="n">
+        <v>4076.190476190476</v>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S27" t="n">
+        <v>8904.761904761905</v>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W27" t="n">
+        <v>8197.619047619048</v>
+      </c>
+      <c r="X27" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="E28" t="n">
@@ -1197,6 +1885,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q28" t="n">
+        <v>2533.333333333333</v>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S28" t="n">
+        <v>7717.460317460317</v>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W28" t="n">
+        <v>3665.079365079365</v>
+      </c>
+      <c r="X28" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="E29" t="n">
@@ -1215,6 +1927,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q29" t="n">
+        <v>7127.777777777777</v>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S29" t="n">
+        <v>17072.22222222222</v>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W29" t="n">
+        <v>1981.746031746032</v>
+      </c>
+      <c r="X29" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="E30" t="n">
@@ -1233,6 +1969,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q30" t="n">
+        <v>3487.301587301587</v>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S30" t="n">
+        <v>15234.12698412698</v>
+      </c>
+      <c r="T30" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W30" t="n">
+        <v>1445.238095238095</v>
+      </c>
+      <c r="X30" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="E31" t="n">
@@ -1251,6 +2011,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q31" t="n">
+        <v>6548.412698412698</v>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S31" t="n">
+        <v>14162.69841269841</v>
+      </c>
+      <c r="T31" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W31" t="n">
+        <v>7534.920634920634</v>
+      </c>
+      <c r="X31" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="E32" t="n">
@@ -1269,6 +2053,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q32" t="n">
+        <v>7227.777777777777</v>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S32" t="n">
+        <v>1176.984126984127</v>
+      </c>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W32" t="n">
+        <v>8411.904761904761</v>
+      </c>
+      <c r="X32" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="E33" t="n">
@@ -1287,6 +2095,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q33" t="n">
+        <v>3080.15873015873</v>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S33" t="n">
+        <v>3011.111111111111</v>
+      </c>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W33" t="n">
+        <v>12134.12698412698</v>
+      </c>
+      <c r="X33" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="E34" t="n">
@@ -1305,6 +2137,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q34" t="n">
+        <v>4114.285714285714</v>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S34" t="n">
+        <v>3455.555555555555</v>
+      </c>
+      <c r="T34" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W34" t="n">
+        <v>5383.333333333333</v>
+      </c>
+      <c r="X34" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="E35" t="n">
@@ -1323,6 +2179,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q35" t="n">
+        <v>1001.587301587302</v>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S35" t="n">
+        <v>14324.60317460317</v>
+      </c>
+      <c r="T35" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W35" t="n">
+        <v>5028.571428571428</v>
+      </c>
+      <c r="X35" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="E36" t="n">
@@ -1341,6 +2221,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q36" t="n">
+        <v>6353.968253968254</v>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S36" t="n">
+        <v>1379.365079365079</v>
+      </c>
+      <c r="T36" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W36" t="n">
+        <v>5415.873015873016</v>
+      </c>
+      <c r="X36" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="E37" t="n">
@@ -1359,6 +2263,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q37" t="n">
+        <v>6873.015873015873</v>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S37" t="n">
+        <v>8179.365079365079</v>
+      </c>
+      <c r="T37" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W37" t="n">
+        <v>4529.36507936508</v>
+      </c>
+      <c r="X37" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="E38" t="n">
@@ -1377,6 +2305,30 @@
           <t>CK1_1_0003.jpg</t>
         </is>
       </c>
+      <c r="Q38" t="n">
+        <v>4780.15873015873</v>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S38" t="n">
+        <v>11720.63492063492</v>
+      </c>
+      <c r="T38" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W38" t="n">
+        <v>5939.68253968254</v>
+      </c>
+      <c r="X38" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="E39" t="n">
@@ -1387,6 +2339,30 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q39" t="n">
+        <v>3204.761904761905</v>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S39" t="n">
+        <v>5464.285714285714</v>
+      </c>
+      <c r="T39" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W39" t="n">
+        <v>7924.603174603174</v>
+      </c>
+      <c r="X39" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="E40" t="n">
@@ -1397,6 +2373,30 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q40" t="n">
+        <v>4736.507936507936</v>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S40" t="n">
+        <v>9470.63492063492</v>
+      </c>
+      <c r="T40" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W40" t="n">
+        <v>5684.920634920634</v>
+      </c>
+      <c r="X40" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="E41" t="n">
@@ -1407,6 +2407,30 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q41" t="n">
+        <v>8258.730158730159</v>
+      </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S41" t="n">
+        <v>4291.269841269841</v>
+      </c>
+      <c r="T41" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W41" t="n">
+        <v>6191.269841269841</v>
+      </c>
+      <c r="X41" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="E42" t="n">
@@ -1417,6 +2441,30 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q42" t="n">
+        <v>5910.31746031746</v>
+      </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S42" t="n">
+        <v>8436.507936507936</v>
+      </c>
+      <c r="T42" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W42" t="n">
+        <v>4869.841269841269</v>
+      </c>
+      <c r="X42" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="E43" t="n">
@@ -1427,6 +2475,30 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q43" t="n">
+        <v>8396.825396825396</v>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S43" t="n">
+        <v>5277.777777777777</v>
+      </c>
+      <c r="T43" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W43" t="n">
+        <v>11004.7619047619</v>
+      </c>
+      <c r="X43" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="E44" t="n">
@@ -1437,6 +2509,30 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q44" t="n">
+        <v>1281.746031746032</v>
+      </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S44" t="n">
+        <v>20223.01587301587</v>
+      </c>
+      <c r="T44" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W44" t="n">
+        <v>4408.730158730158</v>
+      </c>
+      <c r="X44" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="E45" t="n">
@@ -1447,6 +2543,30 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q45" t="n">
+        <v>3803.174603174603</v>
+      </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S45" t="n">
+        <v>2257.936507936508</v>
+      </c>
+      <c r="T45" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W45" t="n">
+        <v>4092.063492063492</v>
+      </c>
+      <c r="X45" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="E46" t="n">
@@ -1457,6 +2577,30 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q46" t="n">
+        <v>5840.47619047619</v>
+      </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S46" t="n">
+        <v>13828.57142857143</v>
+      </c>
+      <c r="T46" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W46" t="n">
+        <v>6703.968253968254</v>
+      </c>
+      <c r="X46" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="E47" t="n">
@@ -1467,6 +2611,30 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q47" t="n">
+        <v>7578.571428571428</v>
+      </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S47" t="n">
+        <v>10344.44444444444</v>
+      </c>
+      <c r="T47" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W47" t="n">
+        <v>3742.063492063492</v>
+      </c>
+      <c r="X47" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="E48" t="n">
@@ -1477,6 +2645,30 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q48" t="n">
+        <v>5010.31746031746</v>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S48" t="n">
+        <v>6281.746031746032</v>
+      </c>
+      <c r="T48" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W48" t="n">
+        <v>3385.714285714285</v>
+      </c>
+      <c r="X48" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="E49" t="n">
@@ -1487,6 +2679,30 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q49" t="n">
+        <v>8007.936507936507</v>
+      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S49" t="n">
+        <v>5580.952380952381</v>
+      </c>
+      <c r="T49" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W49" t="n">
+        <v>1964.285714285714</v>
+      </c>
+      <c r="X49" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="E50" t="n">
@@ -1497,6 +2713,30 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q50" t="n">
+        <v>3692.063492063492</v>
+      </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="S50" t="n">
+        <v>2676.190476190476</v>
+      </c>
+      <c r="T50" t="inlineStr">
+        <is>
+          <t>CK1_1_0004.jpg</t>
+        </is>
+      </c>
+      <c r="W50" t="n">
+        <v>11281.74603174603</v>
+      </c>
+      <c r="X50" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="E51" t="n">
@@ -1507,6 +2747,22 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q51" t="n">
+        <v>4457.936507936508</v>
+      </c>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="W51" t="n">
+        <v>6196.031746031746</v>
+      </c>
+      <c r="X51" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="E52" t="n">
@@ -1517,6 +2773,22 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q52" t="n">
+        <v>5142.857142857142</v>
+      </c>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="W52" t="n">
+        <v>6747.619047619047</v>
+      </c>
+      <c r="X52" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="E53" t="n">
@@ -1527,6 +2799,22 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q53" t="n">
+        <v>5100.79365079365</v>
+      </c>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="W53" t="n">
+        <v>6059.523809523809</v>
+      </c>
+      <c r="X53" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="E54" t="n">
@@ -1537,6 +2825,22 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q54" t="n">
+        <v>3206.349206349206</v>
+      </c>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="W54" t="n">
+        <v>6919.841269841269</v>
+      </c>
+      <c r="X54" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="E55" t="n">
@@ -1547,6 +2851,22 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q55" t="n">
+        <v>1535.714285714286</v>
+      </c>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="W55" t="n">
+        <v>4157.142857142857</v>
+      </c>
+      <c r="X55" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="E56" t="n">
@@ -1557,6 +2877,22 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q56" t="n">
+        <v>4565.079365079365</v>
+      </c>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="W56" t="n">
+        <v>6423.809523809524</v>
+      </c>
+      <c r="X56" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="E57" t="n">
@@ -1567,6 +2903,22 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q57" t="n">
+        <v>3581.746031746031</v>
+      </c>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="W57" t="n">
+        <v>5606.349206349206</v>
+      </c>
+      <c r="X57" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="E58" t="n">
@@ -1577,6 +2929,22 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q58" t="n">
+        <v>4384.126984126984</v>
+      </c>
+      <c r="R58" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="W58" t="n">
+        <v>8192.063492063491</v>
+      </c>
+      <c r="X58" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="E59" t="n">
@@ -1587,6 +2955,22 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q59" t="n">
+        <v>6914.285714285714</v>
+      </c>
+      <c r="R59" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
+      <c r="W59" t="n">
+        <v>10378.57142857143</v>
+      </c>
+      <c r="X59" t="inlineStr">
+        <is>
+          <t>CK1_1_0005.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="E60" t="n">
@@ -1597,6 +2981,14 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q60" t="n">
+        <v>4119.047619047619</v>
+      </c>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="E61" t="n">
@@ -1607,6 +2999,14 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q61" t="n">
+        <v>7615.873015873016</v>
+      </c>
+      <c r="R61" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="E62" t="n">
@@ -1617,6 +3017,14 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q62" t="n">
+        <v>6737.301587301587</v>
+      </c>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="E63" t="n">
@@ -1627,6 +3035,14 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q63" t="n">
+        <v>6050</v>
+      </c>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="E64" t="n">
@@ -1637,6 +3053,14 @@
           <t>CK1_1_0002.jpg</t>
         </is>
       </c>
+      <c r="Q64" t="n">
+        <v>5831.746031746032</v>
+      </c>
+      <c r="R64" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="E65" t="n">
@@ -1645,6 +3069,14 @@
       <c r="F65" t="inlineStr">
         <is>
           <t>CK1_1_0002.jpg</t>
+        </is>
+      </c>
+      <c r="Q65" t="n">
+        <v>4625.396825396825</v>
+      </c>
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>CK1_1_0003.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>